<commit_message>
@Cachelookup and webdriver fire event
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/testdata.xlsx
+++ b/src/main/java/com/crm/qa/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15900" windowHeight="2325"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -40,18 +40,9 @@
     <t>Kalyan</t>
   </si>
   <si>
-    <t>King</t>
-  </si>
-  <si>
-    <t>Singh</t>
-  </si>
-  <si>
     <t>Vamsi</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -62,6 +53,15 @@
   </si>
   <si>
     <t>Dr.</t>
+  </si>
+  <si>
+    <t>King1</t>
+  </si>
+  <si>
+    <t>Singh1</t>
+  </si>
+  <si>
+    <t>Kumar1</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,24 +438,24 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -463,13 +463,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>